<commit_message>
Added train and backprop
</commit_message>
<xml_diff>
--- a/tester/dataxlsx.xlsx
+++ b/tester/dataxlsx.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\nn\tester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\nn\tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
   <si>
     <t>x1</t>
   </si>
@@ -39,9 +39,6 @@
     <t>x3</t>
   </si>
   <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>{</t>
   </si>
   <si>
@@ -51,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +98,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -115,6 +112,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -343,7 +341,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9C86-48E3-A5BC-4887D570531D}"/>
             </c:ext>
@@ -542,7 +540,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9C86-48E3-A5BC-4887D570531D}"/>
             </c:ext>
@@ -556,11 +554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="403932920"/>
-        <c:axId val="403933248"/>
+        <c:axId val="210584696"/>
+        <c:axId val="210587048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="403932920"/>
+        <c:axId val="210584696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,12 +615,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403933248"/>
+        <c:crossAx val="210587048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="403933248"/>
+        <c:axId val="210587048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403932920"/>
+        <c:crossAx val="210584696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -693,6 +691,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1649,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B24"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,409 +2044,270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E23"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="5" max="5" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="B1">
-        <v>0.2</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="D1">
-        <v>1.0205622581941112</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0.43</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>1.2185069075798352</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0.32</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>0.18461747103124537</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0.53</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>1.53472088362903</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0.59</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>0.82231263356048889</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>0.4199229123062711</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>0.76600000000000001</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
-        <v>-0.21660316930374252</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>0.85399999999999998</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
-        <v>-0.58398458496628258</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>1.6982398062237818</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="B10">
-        <v>1.03</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>0.95386304142582834</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="D11">
-        <v>1.8753332870195454</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
-        <v>1.206</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="D12">
-        <v>1.1325482251038421</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
-        <v>1.294</v>
-      </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="D13">
-        <v>2.0583063551943952</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>1.3819999999999999</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="D14">
-        <v>0.2930872564851319</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="B15">
-        <v>1.47</v>
-      </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="D15">
-        <v>0.4442086125524245</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
-        <v>1.5580000000000001</v>
-      </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="D16">
-        <v>1.8921337608132698</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="B17">
-        <v>1.6459999999999999</v>
-      </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="D17">
-        <v>0.99</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="B18">
-        <v>1.734</v>
-      </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="D18">
-        <v>0.93</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
-        <v>1.8220000000000001</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="D19">
-        <v>0.988834473198547</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="B20">
-        <v>1.91</v>
-      </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="D20">
-        <v>0.94874060431523399</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="B21">
-        <v>1.998</v>
-      </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="D21">
-        <v>0.90864673543192198</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="B22">
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>0.86855286654860897</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>5</v>
-      </c>
-      <c r="B23">
-        <v>2.1739999999999999</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>0.82845899766529596</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>